<commit_message>
Table with execution time and statistical confidence
</commit_message>
<xml_diff>
--- a/Docs/Paper/TODAES results.xlsx
+++ b/Docs/Paper/TODAES results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\Dropbox\Doutorado\TODAES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\Documents\ESBMCParallel\Docs\Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t>Exact Solution</t>
   </si>
@@ -89,27 +89,6 @@
   </si>
   <si>
     <t>Error %</t>
-  </si>
-  <si>
-    <t>13.3</t>
-  </si>
-  <si>
-    <t>0.0</t>
-  </si>
-  <si>
-    <t>29.0</t>
-  </si>
-  <si>
-    <t>1.7</t>
-  </si>
-  <si>
-    <t>-6.5</t>
-  </si>
-  <si>
-    <t>-37.6</t>
-  </si>
-  <si>
-    <t>-27.5</t>
   </si>
   <si>
     <r>
@@ -212,10 +191,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
-    <numFmt numFmtId="173" formatCode="#,##0.0000000"/>
-    <numFmt numFmtId="174" formatCode="#,##0.00000000"/>
-    <numFmt numFmtId="178" formatCode="0.0"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="#,##0.0000000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00000000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -338,19 +318,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -359,40 +333,49 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -679,7 +662,7 @@
   <dimension ref="B1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,34 +675,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E1" s="17" t="s">
-        <v>31</v>
+      <c r="E1" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C3" s="8"/>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -777,7 +760,7 @@
     </row>
     <row r="6" spans="2:12" ht="18" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1">
         <v>20</v>
@@ -802,63 +785,63 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="11">
+      <c r="C7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="8">
         <v>15</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="8">
         <v>47</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="8">
         <v>31</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="8">
         <v>241</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="8">
         <v>692</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="8">
         <v>13820</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="8">
         <v>876</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="B8" s="12"/>
-      <c r="C8" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="13">
+      <c r="B8" s="27"/>
+      <c r="C8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="9">
         <v>19</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="9">
         <v>4</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="9">
         <v>19</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="9">
         <v>46</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="9">
         <v>533</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="9">
         <v>4231</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="9">
         <v>297</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -879,7 +862,7 @@
       <c r="H9" s="2">
         <v>1806</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="4" t="s">
         <v>17</v>
       </c>
       <c r="J9" s="2">
@@ -887,9 +870,9 @@
       </c>
     </row>
     <row r="10" spans="2:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="B10" s="6"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D10" s="3">
         <v>15</v>
@@ -906,7 +889,7 @@
       <c r="H10" s="3">
         <v>692</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J10" s="3">
@@ -914,63 +897,63 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="8">
         <v>7</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="8">
         <v>7</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="8">
         <v>9</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="8">
         <v>340</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="8">
         <v>2050</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="8">
         <v>1372</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="8">
         <v>5000</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
-      <c r="C12" s="13" t="s">
+      <c r="B12" s="25"/>
+      <c r="C12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>26</v>
+      <c r="D12" s="29">
+        <v>13.3</v>
+      </c>
+      <c r="E12" s="30">
+        <v>0</v>
+      </c>
+      <c r="F12" s="30">
+        <v>29</v>
+      </c>
+      <c r="G12" s="30">
+        <v>1.7</v>
+      </c>
+      <c r="H12" s="30">
+        <v>-6.5</v>
+      </c>
+      <c r="I12" s="30">
+        <v>-37.6</v>
+      </c>
+      <c r="J12" s="30">
+        <v>-27.5</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="22" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -985,9 +968,9 @@
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="2:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="B14" s="6"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -998,35 +981,35 @@
       <c r="J14" s="3"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
     </row>
     <row r="16" spans="2:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="B16" s="15"/>
-      <c r="C16" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="22" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1041,9 +1024,9 @@
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="2:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="B18" s="6"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1054,77 +1037,77 @@
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
     </row>
     <row r="20" spans="2:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="B20" s="15"/>
-      <c r="C20" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
-        <v>30</v>
+      <c r="B21" s="22" t="s">
+        <v>23</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="16">
         <f>'ESBMC-vZ'!H6</f>
         <v>0.29458093643333333</v>
       </c>
-      <c r="E21" s="23">
+      <c r="E21" s="16">
         <f>'ESBMC-vZ'!H5</f>
         <v>0.31701231000000002</v>
       </c>
-      <c r="F21" s="23">
+      <c r="F21" s="16">
         <f>'ESBMC-vZ'!H7</f>
         <v>0.66174101829999998</v>
       </c>
-      <c r="G21" s="23">
+      <c r="G21" s="16">
         <f>'ESBMC-vZ'!H8</f>
         <v>86.371642669999986</v>
       </c>
-      <c r="H21" s="5" t="str">
+      <c r="H21" s="4" t="str">
         <f>'ESBMC-vZ'!D9</f>
         <v>TO</v>
       </c>
-      <c r="I21" s="5" t="str">
+      <c r="I21" s="4" t="str">
         <f>'ESBMC-vZ'!D10</f>
         <v>TO</v>
       </c>
-      <c r="J21" s="5" t="str">
+      <c r="J21" s="4" t="str">
         <f>'ESBMC-vZ'!D11</f>
         <v>TO</v>
       </c>
-      <c r="L21" s="22">
+      <c r="L21" s="15">
         <f>'ESBMC-vZ'!L8</f>
         <v>0.92</v>
       </c>
     </row>
     <row r="22" spans="2:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="B22" s="6"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D22" s="3">
         <f>'ESBMC-vZ'!C6</f>
@@ -1158,6 +1141,7 @@
     <mergeCell ref="B19:B20"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1234,72 +1218,72 @@
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K2" s="18"/>
-      <c r="L2" s="19"/>
+        <v>37</v>
+      </c>
+      <c r="K2" s="11"/>
+      <c r="L2" s="12"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="17"/>
+      <c r="C4" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
-      <c r="C4" s="26" t="s">
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="K4" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="L4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L4" t="s">
-        <v>45</v>
-      </c>
-      <c r="M4" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="17">
         <v>47</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="17">
         <v>0.3183119297</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="17">
         <v>0.31364393229999998</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="17">
         <v>0.31908106800000002</v>
       </c>
       <c r="H5">
@@ -1317,7 +1301,7 @@
       <c r="K5">
         <v>0.08</v>
       </c>
-      <c r="L5" s="19">
+      <c r="L5" s="12">
         <f>1-K5</f>
         <v>0.92</v>
       </c>
@@ -1327,19 +1311,19 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="17">
         <v>15</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="17">
         <v>0.29760599139999999</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="17">
         <v>0.29183483119999998</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="17">
         <v>0.29430198670000002</v>
       </c>
       <c r="H6">
@@ -1357,7 +1341,7 @@
       <c r="K6">
         <v>0.08</v>
       </c>
-      <c r="L6" s="19">
+      <c r="L6" s="12">
         <f>1-K6</f>
         <v>0.92</v>
       </c>
@@ -1367,19 +1351,19 @@
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="25">
+      <c r="B7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="17">
         <v>31</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="17">
         <v>0.67384290700000005</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="17">
         <v>0.65836405750000004</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="17">
         <v>0.65301609039999997</v>
       </c>
       <c r="H7">
@@ -1397,7 +1381,7 @@
       <c r="K7">
         <v>0.08</v>
       </c>
-      <c r="L7" s="19">
+      <c r="L7" s="12">
         <f>1-K7</f>
         <v>0.92</v>
       </c>
@@ -1407,19 +1391,19 @@
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="17">
         <v>241</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="19">
         <v>84.589081050000004</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="20">
         <v>85.896725889999999</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="20">
         <v>88.629121069999997</v>
       </c>
       <c r="H8">
@@ -1437,7 +1421,7 @@
       <c r="K8">
         <v>0.08</v>
       </c>
-      <c r="L8" s="19">
+      <c r="L8" s="12">
         <f>1-K8</f>
         <v>0.92</v>
       </c>
@@ -1447,52 +1431,52 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="G16" s="20"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="7:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="G17" s="21"/>
+      <c r="G17" s="14"/>
     </row>
     <row r="18" spans="7:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="H18" s="21"/>
+      <c r="H18" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Table with statistical confidence and all the times taken 3 times
</commit_message>
<xml_diff>
--- a/Docs/Paper/TODAES results.xlsx
+++ b/Docs/Paper/TODAES results.xlsx
@@ -12,13 +12,16 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Tempos Consolidados" sheetId="6" r:id="rId1"/>
+    <sheet name="Summary" sheetId="6" r:id="rId1"/>
     <sheet name="ESBMC" sheetId="1" r:id="rId2"/>
     <sheet name="ESBMC-SS" sheetId="2" r:id="rId3"/>
     <sheet name="ESBMC-PS" sheetId="3" r:id="rId4"/>
     <sheet name="ESBMC-PB" sheetId="4" r:id="rId5"/>
     <sheet name="ESBMC-vZ" sheetId="5" r:id="rId6"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="46">
   <si>
     <t>Exact Solution</t>
   </si>
@@ -142,9 +145,6 @@
     <t>ESBMC-vZ</t>
   </si>
   <si>
-    <t>Tabela com os tempos consolidados</t>
-  </si>
-  <si>
     <t>TODAES – vZ</t>
   </si>
   <si>
@@ -185,17 +185,42 @@
   </si>
   <si>
     <t>Statistical confidence</t>
+  </si>
+  <si>
+    <t>TODAES – ESBMC Loop Sequential</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>TODAES – ESBMC Parallel (ESBMC-SS)</t>
+  </si>
+  <si>
+    <t>MO= 15GB, TO=7200s</t>
+  </si>
+  <si>
+    <t>TODAES – Paralle Sequential (ESBMC-PS)</t>
+  </si>
+  <si>
+    <t>TODAES – Parallel Binary (ESBMC-PB)</t>
+  </si>
+  <si>
+    <t>Summary of Results</t>
+  </si>
+  <si>
+    <t>MO = 15GB, TO=7200s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="#,##0.0000000"/>
     <numFmt numFmtId="165" formatCode="#,##0.00000000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="#,##0.0"/>
+    <numFmt numFmtId="172" formatCode="0.0%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -261,7 +286,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -313,12 +338,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -340,7 +374,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -349,6 +382,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -372,10 +408,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="172" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -394,6 +448,37 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sumário"/>
+      <sheetName val="tabela vertical"/>
+      <sheetName val="ESBMC Multi-core"/>
+      <sheetName val="ESBMC invariantes"/>
+      <sheetName val="ILP GA"/>
+      <sheetName val="memoria GA"/>
+      <sheetName val="Memoria ILP"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5">
+        <row r="79">
+          <cell r="A79">
+            <v>0.91700000000000004</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="6"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -659,27 +744,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L22"/>
+  <dimension ref="B1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="11.28515625" style="1" customWidth="1"/>
-    <col min="3" max="11" width="9.140625" style="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="6" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="9.140625" style="1"/>
     <col min="12" max="12" width="21.5703125" style="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
@@ -705,6 +790,9 @@
       <c r="J3" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="L3" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
@@ -848,25 +936,28 @@
         <v>16</v>
       </c>
       <c r="D9" s="2">
-        <v>2</v>
+        <v>1.57</v>
       </c>
       <c r="E9" s="2">
-        <v>1</v>
+        <v>1.27</v>
       </c>
       <c r="F9" s="2">
-        <v>2</v>
+        <v>1.61</v>
       </c>
       <c r="G9" s="2">
-        <v>649</v>
+        <v>648.9</v>
       </c>
       <c r="H9" s="2">
-        <v>1806</v>
+        <v>1806.2</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>17</v>
       </c>
       <c r="J9" s="2">
-        <v>5429</v>
+        <v>5429.18</v>
+      </c>
+      <c r="L9" s="36">
+        <v>0.92</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="18" x14ac:dyDescent="0.35">
@@ -903,26 +994,30 @@
       <c r="C11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="8">
-        <v>7</v>
-      </c>
-      <c r="E11" s="8">
-        <v>7</v>
-      </c>
-      <c r="F11" s="8">
-        <v>9</v>
-      </c>
-      <c r="G11" s="8">
-        <v>340</v>
-      </c>
-      <c r="H11" s="8">
+      <c r="D11" s="40">
+        <v>6.69</v>
+      </c>
+      <c r="E11" s="40">
+        <v>7.41</v>
+      </c>
+      <c r="F11" s="40">
+        <v>8.81</v>
+      </c>
+      <c r="G11" s="40">
+        <v>340.39</v>
+      </c>
+      <c r="H11" s="40">
         <v>2050</v>
       </c>
-      <c r="I11" s="8">
-        <v>1372</v>
-      </c>
-      <c r="J11" s="8">
-        <v>5000</v>
+      <c r="I11" s="40">
+        <v>1371.913</v>
+      </c>
+      <c r="J11" s="40">
+        <v>5000.47</v>
+      </c>
+      <c r="L11" s="36">
+        <f>'[1]memoria GA'!$A$79</f>
+        <v>0.91700000000000004</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
@@ -930,25 +1025,25 @@
       <c r="C12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="21">
         <v>13.3</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="21">
         <v>0</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="21">
         <v>29</v>
       </c>
-      <c r="G12" s="30">
+      <c r="G12" s="21">
         <v>1.7</v>
       </c>
-      <c r="H12" s="30">
+      <c r="H12" s="21">
         <v>-6.5</v>
       </c>
-      <c r="I12" s="30">
+      <c r="I12" s="21">
         <v>-37.6</v>
       </c>
-      <c r="J12" s="30">
+      <c r="J12" s="21">
         <v>-27.5</v>
       </c>
     </row>
@@ -959,26 +1054,68 @@
       <c r="C13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="D13" s="15">
+        <f>ESBMC!H6</f>
+        <v>30.333333333333332</v>
+      </c>
+      <c r="E13" s="15">
+        <f>ESBMC!H5</f>
+        <v>313.66666666666669</v>
+      </c>
+      <c r="F13" s="15">
+        <f>ESBMC!H7</f>
+        <v>324.66666666666669</v>
+      </c>
+      <c r="G13" s="4" t="str">
+        <f>ESBMC!H8</f>
+        <v>MO</v>
+      </c>
+      <c r="H13" s="4" t="str">
+        <f>ESBMC!H9</f>
+        <v>MO</v>
+      </c>
+      <c r="I13" s="4" t="str">
+        <f>ESBMC!H10</f>
+        <v>MO</v>
+      </c>
+      <c r="J13" s="4" t="str">
+        <f>ESBMC!H11</f>
+        <v>MO</v>
+      </c>
+      <c r="L13" s="37">
+        <f>ESBMC!L8</f>
+        <v>0.91700000000000015</v>
+      </c>
     </row>
     <row r="14" spans="2:12" ht="18" x14ac:dyDescent="0.35">
       <c r="B14" s="23"/>
       <c r="C14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="D14" s="3">
+        <f>ESBMC!C6</f>
+        <v>15</v>
+      </c>
+      <c r="E14" s="3">
+        <f>ESBMC!C5</f>
+        <v>47</v>
+      </c>
+      <c r="F14" s="3">
+        <f>ESBMC!C7</f>
+        <v>31</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="24" t="s">
@@ -987,26 +1124,69 @@
       <c r="C15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
+      <c r="D15" s="40">
+        <f>'ESBMC-SS'!H6</f>
+        <v>2.2023333333333333</v>
+      </c>
+      <c r="E15" s="40">
+        <f>'ESBMC-SS'!H5</f>
+        <v>5.8263333333333334</v>
+      </c>
+      <c r="F15" s="40">
+        <f>'ESBMC-SS'!H7</f>
+        <v>6.9750000000000005</v>
+      </c>
+      <c r="G15" s="40">
+        <f>'ESBMC-SS'!H8</f>
+        <v>1609.3333333333333</v>
+      </c>
+      <c r="H15" s="41" t="str">
+        <f>'ESBMC-SS'!H9</f>
+        <v>TO</v>
+      </c>
+      <c r="I15" s="41" t="str">
+        <f>'ESBMC-SS'!H10</f>
+        <v>TO</v>
+      </c>
+      <c r="J15" s="41" t="str">
+        <f>'ESBMC-SS'!H11</f>
+        <v>TO</v>
+      </c>
+      <c r="L15" s="37">
+        <f>'ESBMC-SS'!L9</f>
+        <v>0.91700000000000004</v>
+      </c>
     </row>
     <row r="16" spans="2:12" ht="18" x14ac:dyDescent="0.35">
       <c r="B16" s="25"/>
       <c r="C16" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
+      <c r="D16" s="9">
+        <f>'ESBMC-SS'!C6</f>
+        <v>15</v>
+      </c>
+      <c r="E16" s="9">
+        <f>'ESBMC-SS'!C5</f>
+        <v>47</v>
+      </c>
+      <c r="F16" s="9">
+        <f>'ESBMC-SS'!C7</f>
+        <v>31</v>
+      </c>
+      <c r="G16" s="9">
+        <f>'ESBMC-SS'!C8</f>
+        <v>241</v>
+      </c>
+      <c r="H16" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="42" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="22" t="s">
@@ -1015,26 +1195,69 @@
       <c r="C17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="D17" s="15">
+        <f>'ESBMC-PS'!H6</f>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="E17" s="15">
+        <f>'ESBMC-PS'!H5</f>
+        <v>10</v>
+      </c>
+      <c r="F17" s="15">
+        <f>'ESBMC-PS'!H7</f>
+        <v>12</v>
+      </c>
+      <c r="G17" s="15">
+        <f>'ESBMC-PS'!H8</f>
+        <v>2468</v>
+      </c>
+      <c r="H17" s="4" t="str">
+        <f>'ESBMC-PS'!H9</f>
+        <v>TO</v>
+      </c>
+      <c r="I17" s="4" t="str">
+        <f>'ESBMC-PS'!H10</f>
+        <v>TO</v>
+      </c>
+      <c r="J17" s="4" t="str">
+        <f>'ESBMC-PS'!H11</f>
+        <v>TO</v>
+      </c>
+      <c r="L17" s="37">
+        <f>'ESBMC-PS'!L9</f>
+        <v>0.95849999999999991</v>
+      </c>
     </row>
     <row r="18" spans="2:12" ht="18" x14ac:dyDescent="0.35">
       <c r="B18" s="23"/>
       <c r="C18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="D18" s="3">
+        <f>'ESBMC-PS'!C6</f>
+        <v>15</v>
+      </c>
+      <c r="E18" s="3">
+        <f>'ESBMC-PS'!C5</f>
+        <v>47</v>
+      </c>
+      <c r="F18" s="3">
+        <f>'ESBMC-PS'!C7</f>
+        <v>31</v>
+      </c>
+      <c r="G18" s="3">
+        <f>'ESBMC-PS'!C8</f>
+        <v>241</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="24" t="s">
@@ -1043,26 +1266,69 @@
       <c r="C19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
+      <c r="D19" s="40">
+        <f>'ESBMC-PB'!H6</f>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="E19" s="40">
+        <f>'ESBMC-PB'!H5</f>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="F19" s="40">
+        <f>'ESBMC-PB'!H7</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="G19" s="40">
+        <f>'ESBMC-PB'!H8</f>
+        <v>218.66666666666666</v>
+      </c>
+      <c r="H19" s="41" t="str">
+        <f>'ESBMC-PB'!H9</f>
+        <v>TO</v>
+      </c>
+      <c r="I19" s="41" t="str">
+        <f>'ESBMC-PB'!H10</f>
+        <v>TO</v>
+      </c>
+      <c r="J19" s="41" t="str">
+        <f>'ESBMC-PB'!H11</f>
+        <v>TO</v>
+      </c>
+      <c r="L19" s="37">
+        <f>'ESBMC-PB'!L9</f>
+        <v>0.91700000000000004</v>
+      </c>
     </row>
     <row r="20" spans="2:12" ht="18" x14ac:dyDescent="0.35">
       <c r="B20" s="25"/>
       <c r="C20" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
+      <c r="D20" s="9">
+        <f>'ESBMC-PB'!C6</f>
+        <v>15</v>
+      </c>
+      <c r="E20" s="9">
+        <f>'ESBMC-PB'!C5</f>
+        <v>47</v>
+      </c>
+      <c r="F20" s="9">
+        <f>'ESBMC-PB'!C7</f>
+        <v>31</v>
+      </c>
+      <c r="G20" s="9">
+        <f>'ESBMC-PB'!C8</f>
+        <v>241</v>
+      </c>
+      <c r="H20" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="42" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="22" t="s">
@@ -1071,19 +1337,19 @@
       <c r="C21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="15">
         <f>'ESBMC-vZ'!H6</f>
         <v>0.29458093643333333</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="15">
         <f>'ESBMC-vZ'!H5</f>
         <v>0.31701231000000002</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F21" s="15">
         <f>'ESBMC-vZ'!H7</f>
         <v>0.66174101829999998</v>
       </c>
-      <c r="G21" s="16">
+      <c r="G21" s="15">
         <f>'ESBMC-vZ'!H8</f>
         <v>86.371642669999986</v>
       </c>
@@ -1099,9 +1365,9 @@
         <f>'ESBMC-vZ'!D11</f>
         <v>TO</v>
       </c>
-      <c r="L21" s="15">
+      <c r="L21" s="36">
         <f>'ESBMC-vZ'!L8</f>
-        <v>0.92</v>
+        <v>0.91700000000000004</v>
       </c>
     </row>
     <row r="22" spans="2:12" ht="18" x14ac:dyDescent="0.35">
@@ -1125,9 +1391,20 @@
         <f>'ESBMC-vZ'!C8</f>
         <v>241</v>
       </c>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
+      <c r="H22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H24" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1147,60 +1424,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="H9" sqref="H9:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,20 +1444,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K2" s="11"/>
       <c r="L2" s="12"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
@@ -1238,52 +1468,1305 @@
       <c r="F3" s="28"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="17"/>
-      <c r="C4" s="18" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="F4" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="16">
+        <v>47</v>
+      </c>
+      <c r="D5" s="16">
+        <v>342</v>
+      </c>
+      <c r="E5" s="16">
+        <v>293</v>
+      </c>
+      <c r="F5" s="16">
+        <v>306</v>
+      </c>
+      <c r="H5">
+        <f>AVERAGE(D5:F5)</f>
+        <v>313.66666666666669</v>
+      </c>
+      <c r="I5">
+        <f>_xlfn.STDEV.S(D5:F5)</f>
+        <v>25.383721817994566</v>
+      </c>
+      <c r="J5">
+        <f>_xlfn.CONFIDENCE.NORM(K5,I5,3)</f>
+        <v>25.405524451136962</v>
+      </c>
+      <c r="K5">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L5" s="32">
+        <f>1-K5</f>
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="M5" t="str">
+        <f>IF(I5&gt;J5,"NOK","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="16">
+        <v>15</v>
+      </c>
+      <c r="D6" s="16">
+        <v>32</v>
+      </c>
+      <c r="E6" s="16">
+        <v>27</v>
+      </c>
+      <c r="F6" s="16">
+        <v>32</v>
+      </c>
+      <c r="H6">
+        <f>AVERAGE(D6:F6)</f>
+        <v>30.333333333333332</v>
+      </c>
+      <c r="I6">
+        <f>_xlfn.STDEV.S(D6:F6)</f>
+        <v>2.8867513459481291</v>
+      </c>
+      <c r="J6">
+        <f>_xlfn.CONFIDENCE.NORM(K6,I6,3)</f>
+        <v>2.8892308397363253</v>
+      </c>
+      <c r="K6">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L6" s="32">
+        <f>1-K6</f>
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="M6" t="str">
+        <f>IF(I6&gt;J6,"NOK","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
         <v>29</v>
       </c>
+      <c r="C7" s="16">
+        <v>31</v>
+      </c>
+      <c r="D7" s="16">
+        <v>297</v>
+      </c>
+      <c r="E7" s="16">
+        <v>319</v>
+      </c>
+      <c r="F7" s="16">
+        <v>358</v>
+      </c>
+      <c r="H7">
+        <f>AVERAGE(D7:F7)</f>
+        <v>324.66666666666669</v>
+      </c>
+      <c r="I7">
+        <f>_xlfn.STDEV.S(D7:F7)</f>
+        <v>30.892285984260429</v>
+      </c>
+      <c r="J7">
+        <f>_xlfn.CONFIDENCE.NORM(K7,I7,3)</f>
+        <v>30.918820043492328</v>
+      </c>
+      <c r="K7">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L7" s="32">
+        <f>1-K7</f>
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="M7" t="str">
+        <f>IF(I7&gt;J7,"NOK","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="35">
+        <f>AVERAGE(L5:L7)</f>
+        <v>0.91700000000000015</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="7:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="7:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="H18" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:M18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="11"/>
+      <c r="L2" s="12"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>28</v>
+      </c>
       <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
         <v>32</v>
       </c>
+      <c r="K4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="16">
+        <v>47</v>
+      </c>
+      <c r="D5" s="16">
+        <v>5.8230000000000004</v>
+      </c>
+      <c r="E5" s="16">
+        <v>5.8630000000000004</v>
+      </c>
+      <c r="F5" s="16">
+        <v>5.7930000000000001</v>
+      </c>
+      <c r="H5">
+        <f>AVERAGE(D5:F5)</f>
+        <v>5.8263333333333334</v>
+      </c>
+      <c r="I5">
+        <f>_xlfn.STDEV.S(D5:F5)</f>
+        <v>3.5118845842842597E-2</v>
+      </c>
+      <c r="J5">
+        <f>_xlfn.CONFIDENCE.NORM(K5,I5,3)</f>
+        <v>3.5149010186660494E-2</v>
+      </c>
+      <c r="K5">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L5" s="32">
+        <f>1-K5</f>
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="M5" t="str">
+        <f>IF(I5&gt;J5,"NOK","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="16">
+        <v>15</v>
+      </c>
+      <c r="D6" s="16">
+        <v>2.2069999999999999</v>
+      </c>
+      <c r="E6" s="16">
+        <v>2.206</v>
+      </c>
+      <c r="F6" s="16">
+        <v>2.194</v>
+      </c>
+      <c r="H6">
+        <f>AVERAGE(D6:F6)</f>
+        <v>2.2023333333333333</v>
+      </c>
+      <c r="I6">
+        <f>_xlfn.STDEV.S(D6:F6)</f>
+        <v>7.2341781380702054E-3</v>
+      </c>
+      <c r="J6">
+        <f>_xlfn.CONFIDENCE.NORM(K6,I6,3)</f>
+        <v>7.2403917316937877E-3</v>
+      </c>
+      <c r="K6">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L6" s="32">
+        <f>1-K6</f>
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="M6" t="str">
+        <f>IF(I6&gt;J6,"NOK","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="16">
+        <v>31</v>
+      </c>
+      <c r="D7" s="16">
+        <v>7.0309999999999997</v>
+      </c>
+      <c r="E7" s="16">
+        <v>7.0750000000000002</v>
+      </c>
+      <c r="F7" s="16">
+        <v>6.819</v>
+      </c>
+      <c r="H7">
+        <f>AVERAGE(D7:F7)</f>
+        <v>6.9750000000000005</v>
+      </c>
+      <c r="I7">
+        <f>_xlfn.STDEV.S(D7:F7)</f>
+        <v>0.13687950905814941</v>
+      </c>
+      <c r="J7">
+        <f>_xlfn.CONFIDENCE.NORM(K7,I7,3)</f>
+        <v>0.13699707785842638</v>
+      </c>
+      <c r="K7">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L7" s="32">
+        <f>1-K7</f>
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="M7" t="str">
+        <f>IF(I7&gt;J7,"NOK","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="16">
+        <v>241</v>
+      </c>
+      <c r="D8" s="31">
+        <v>1605</v>
+      </c>
+      <c r="E8" s="31">
+        <v>1620</v>
+      </c>
+      <c r="F8" s="31">
+        <v>1603</v>
+      </c>
+      <c r="H8">
+        <f>AVERAGE(D8:F8)</f>
+        <v>1609.3333333333333</v>
+      </c>
+      <c r="I8">
+        <f>_xlfn.STDEV.S(D8:F8)</f>
+        <v>9.2915732431775684</v>
+      </c>
+      <c r="J8">
+        <f>_xlfn.CONFIDENCE.NORM(K8,I8,3)</f>
+        <v>9.2995539783979275</v>
+      </c>
+      <c r="K8">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L8" s="32">
+        <f>1-K8</f>
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="M8" t="str">
+        <f>IF(I8&gt;J8,"NOK","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="34">
+        <f>AVERAGE(L5:L8)</f>
+        <v>0.91700000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="7:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="7:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="H18" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:M18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="11"/>
+      <c r="L2" s="12"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
       <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="16">
+        <v>47</v>
+      </c>
+      <c r="D5" s="16">
+        <v>10</v>
+      </c>
+      <c r="E5" s="16">
+        <v>10</v>
+      </c>
+      <c r="F5" s="16">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <f>AVERAGE(D5:F5)</f>
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <f>_xlfn.STDEV.S(D5:F5)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" t="e">
+        <f>_xlfn.CONFIDENCE.NORM(K5,I5,3)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K5">
+        <v>0.08</v>
+      </c>
+      <c r="L5" s="12">
+        <v>1</v>
+      </c>
+      <c r="M5" t="e">
+        <f>IF(I5&gt;J5,"NOK","OK")</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="16">
+        <v>15</v>
+      </c>
+      <c r="D6" s="16">
+        <v>3</v>
+      </c>
+      <c r="E6" s="16">
+        <v>4</v>
+      </c>
+      <c r="F6" s="16">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <f>AVERAGE(D6:F6)</f>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="I6">
+        <f>_xlfn.STDEV.S(D6:F6)</f>
+        <v>0.57735026918962473</v>
+      </c>
+      <c r="J6">
+        <f>_xlfn.CONFIDENCE.NORM(K6,I6,3)</f>
+        <v>0.57784616794726396</v>
+      </c>
+      <c r="K6">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L6" s="32">
+        <f>1-K6</f>
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="M6" t="str">
+        <f>IF(I6&gt;J6,"NOK","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="16">
         <v>31</v>
       </c>
+      <c r="D7" s="16">
+        <v>12</v>
+      </c>
+      <c r="E7" s="16">
+        <v>12</v>
+      </c>
+      <c r="F7" s="16">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <f>AVERAGE(D7:F7)</f>
+        <v>12</v>
+      </c>
+      <c r="I7">
+        <f>_xlfn.STDEV.S(D7:F7)</f>
+        <v>0</v>
+      </c>
+      <c r="J7" t="e">
+        <f>_xlfn.CONFIDENCE.NORM(K7,I7,3)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K7">
+        <v>0.08</v>
+      </c>
+      <c r="L7" s="12">
+        <v>1</v>
+      </c>
+      <c r="M7" t="e">
+        <f>IF(I7&gt;J7,"NOK","OK")</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="16">
+        <v>241</v>
+      </c>
+      <c r="D8" s="31">
+        <v>2482</v>
+      </c>
+      <c r="E8" s="31">
+        <v>2478</v>
+      </c>
+      <c r="F8" s="31">
+        <v>2444</v>
+      </c>
+      <c r="H8">
+        <f>AVERAGE(D8:F8)</f>
+        <v>2468</v>
+      </c>
+      <c r="I8">
+        <f>_xlfn.STDEV.S(D8:F8)</f>
+        <v>20.880613017821101</v>
+      </c>
+      <c r="J8">
+        <f>_xlfn.CONFIDENCE.NORM(K8,I8,3)</f>
+        <v>20.898547832450735</v>
+      </c>
+      <c r="K8">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L8" s="32">
+        <f>1-K8</f>
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="M8" t="str">
+        <f>IF(I8&gt;J8,"NOK","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="33">
+        <f>AVERAGE(L5:L8)</f>
+        <v>0.95849999999999991</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="7:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="7:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="H18" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:M18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="11"/>
+      <c r="L2" s="12"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
       <c r="J4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
         <v>33</v>
       </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="16">
+        <v>47</v>
+      </c>
+      <c r="D5" s="16">
+        <v>5</v>
+      </c>
+      <c r="E5" s="16">
+        <v>4</v>
+      </c>
+      <c r="F5" s="16">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <f>AVERAGE(D5:F5)</f>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="I5">
+        <f>_xlfn.STDEV.S(D5:F5)</f>
+        <v>0.57735026918962784</v>
+      </c>
+      <c r="J5">
+        <f>_xlfn.CONFIDENCE.NORM(K5,I5,3)</f>
+        <v>0.57784616794726706</v>
+      </c>
+      <c r="K5">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L5" s="32">
+        <f>1-K5</f>
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="M5" t="str">
+        <f>IF(I5&gt;J5,"NOK","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="16">
+        <v>15</v>
+      </c>
+      <c r="D6" s="16">
+        <v>5</v>
+      </c>
+      <c r="E6" s="16">
+        <v>4</v>
+      </c>
+      <c r="F6" s="16">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <f>AVERAGE(D6:F6)</f>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="I6">
+        <f>_xlfn.STDEV.S(D6:F6)</f>
+        <v>0.57735026918962473</v>
+      </c>
+      <c r="J6">
+        <f>_xlfn.CONFIDENCE.NORM(K6,I6,3)</f>
+        <v>0.57784616794726396</v>
+      </c>
+      <c r="K6">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L6" s="32">
+        <f>1-K6</f>
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="M6" t="str">
+        <f>IF(I6&gt;J6,"NOK","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="16">
+        <v>31</v>
+      </c>
+      <c r="D7" s="16">
+        <v>7</v>
+      </c>
+      <c r="E7" s="16">
+        <v>6</v>
+      </c>
+      <c r="F7" s="16">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <f>AVERAGE(D7:F7)</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="I7">
+        <f>_xlfn.STDEV.S(D7:F7)</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="J7">
+        <f>_xlfn.CONFIDENCE.NORM(K7,I7,3)</f>
+        <v>0.57784616794726507</v>
+      </c>
+      <c r="K7">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L7" s="32">
+        <f>1-K7</f>
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="M7" t="str">
+        <f>IF(I7&gt;J7,"NOK","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="16">
+        <v>241</v>
+      </c>
+      <c r="D8" s="30">
+        <v>215</v>
+      </c>
+      <c r="E8" s="30">
+        <v>220</v>
+      </c>
+      <c r="F8" s="30">
+        <v>221</v>
+      </c>
+      <c r="H8">
+        <f>AVERAGE(D8:F8)</f>
+        <v>218.66666666666666</v>
+      </c>
+      <c r="I8">
+        <f>_xlfn.STDEV.S(D8:F8)</f>
+        <v>3.2145502536643185</v>
+      </c>
+      <c r="J8">
+        <f>_xlfn.CONFIDENCE.NORM(K8,I8,3)</f>
+        <v>3.2173113010946741</v>
+      </c>
+      <c r="K8">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L8" s="32">
+        <f>1-K8</f>
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="M8" t="str">
+        <f>IF(I8&gt;J8,"NOK","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="34">
+        <f>AVERAGE(L5:L8)</f>
+        <v>0.91700000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="7:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="7:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="H18" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:M18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="11"/>
+      <c r="L2" s="12"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
       <c r="K4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" t="s">
         <v>34</v>
       </c>
-      <c r="L4" t="s">
-        <v>38</v>
-      </c>
-      <c r="M4" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="16">
         <v>47</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="16">
         <v>0.3183119297</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="16">
         <v>0.31364393229999998</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="16">
         <v>0.31908106800000002</v>
       </c>
       <c r="H5">
@@ -1296,14 +2779,14 @@
       </c>
       <c r="J5">
         <f>_xlfn.CONFIDENCE.NORM(K5,I5,3)</f>
-        <v>2.9739977145837172E-3</v>
+        <v>2.9448680909884093E-3</v>
       </c>
       <c r="K5">
-        <v>0.08</v>
-      </c>
-      <c r="L5" s="12">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L5" s="32">
         <f>1-K5</f>
-        <v>0.92</v>
+        <v>0.91700000000000004</v>
       </c>
       <c r="M5" t="str">
         <f>IF(I5&gt;J5,"NOK","OK")</f>
@@ -1311,19 +2794,19 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="16">
         <v>15</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="16">
         <v>0.29760599139999999</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <v>0.29183483119999998</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="16">
         <v>0.29430198670000002</v>
       </c>
       <c r="H6">
@@ -1336,14 +2819,14 @@
       </c>
       <c r="J6">
         <f>_xlfn.CONFIDENCE.NORM(K6,I6,3)</f>
-        <v>2.9268295253172733E-3</v>
+        <v>2.8981619032871536E-3</v>
       </c>
       <c r="K6">
-        <v>0.08</v>
-      </c>
-      <c r="L6" s="12">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L6" s="32">
         <f>1-K6</f>
-        <v>0.92</v>
+        <v>0.91700000000000004</v>
       </c>
       <c r="M6" t="str">
         <f>IF(I6&gt;J6,"NOK","OK")</f>
@@ -1351,19 +2834,19 @@
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="17">
+      <c r="B7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="16">
         <v>31</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="16">
         <v>0.67384290700000005</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="16">
         <v>0.65836405750000004</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="16">
         <v>0.65301609039999997</v>
       </c>
       <c r="H7">
@@ -1376,14 +2859,14 @@
       </c>
       <c r="J7">
         <f>_xlfn.CONFIDENCE.NORM(K7,I7,3)</f>
-        <v>1.093265585216514E-2</v>
+        <v>1.0825573002602432E-2</v>
       </c>
       <c r="K7">
-        <v>0.08</v>
-      </c>
-      <c r="L7" s="12">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L7" s="32">
         <f>1-K7</f>
-        <v>0.92</v>
+        <v>0.91700000000000004</v>
       </c>
       <c r="M7" t="str">
         <f>IF(I7&gt;J7,"NOK","OK")</f>
@@ -1391,19 +2874,19 @@
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="16">
         <v>241</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="18">
         <v>84.589081050000004</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="19">
         <v>85.896725889999999</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="19">
         <v>88.629121069999997</v>
       </c>
       <c r="H8">
@@ -1416,14 +2899,14 @@
       </c>
       <c r="J8">
         <f>_xlfn.CONFIDENCE.NORM(K8,I8,3)</f>
-        <v>2.0836450329908813</v>
+        <v>2.063236209130789</v>
       </c>
       <c r="K8">
-        <v>0.08</v>
-      </c>
-      <c r="L8" s="12">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L8" s="32">
         <f>1-K8</f>
-        <v>0.92</v>
+        <v>0.91700000000000004</v>
       </c>
       <c r="M8" t="str">
         <f>IF(I8&gt;J8,"NOK","OK")</f>
@@ -1431,43 +2914,68 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
+      <c r="C9" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="34">
+        <f>AVERAGE(L5:L8)</f>
+        <v>0.91700000000000004</v>
+      </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
+      <c r="C10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
+      <c r="C11" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="G16" s="13"/>

</xml_diff>

<commit_message>
IJES templates and guides
</commit_message>
<xml_diff>
--- a/Docs/Paper/TODAES results.xlsx
+++ b/Docs/Paper/TODAES results.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
-    <sheet name="ESBMC" sheetId="1" r:id="rId2"/>
-    <sheet name="ESBMC-SS" sheetId="2" r:id="rId3"/>
-    <sheet name="ESBMC-PS" sheetId="3" r:id="rId4"/>
-    <sheet name="ESBMC-PB" sheetId="4" r:id="rId5"/>
-    <sheet name="ESBMC-vZ" sheetId="5" r:id="rId6"/>
+    <sheet name="Summary TO=3600s" sheetId="7" r:id="rId2"/>
+    <sheet name="ESBMC" sheetId="1" r:id="rId3"/>
+    <sheet name="ESBMC-SS" sheetId="2" r:id="rId4"/>
+    <sheet name="ESBMC-PS" sheetId="3" r:id="rId5"/>
+    <sheet name="ESBMC-PB" sheetId="4" r:id="rId6"/>
+    <sheet name="ESBMC-vZ" sheetId="5" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="46">
   <si>
     <t>Exact Solution</t>
   </si>
@@ -220,7 +221,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00000000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="#,##0.0"/>
-    <numFmt numFmtId="172" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -352,7 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -387,6 +388,30 @@
     <xf numFmtId="167" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -408,28 +433,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -746,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A6" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,7 +877,7 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="40" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -902,7 +906,7 @@
       </c>
     </row>
     <row r="8" spans="2:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="B8" s="27"/>
+      <c r="B8" s="41"/>
       <c r="C8" s="9" t="s">
         <v>22</v>
       </c>
@@ -929,7 +933,7 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -956,12 +960,12 @@
       <c r="J9" s="2">
         <v>5429.18</v>
       </c>
-      <c r="L9" s="36">
+      <c r="L9" s="29">
         <v>0.92</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="B10" s="23"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="3" t="s">
         <v>21</v>
       </c>
@@ -988,40 +992,40 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="38" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="33">
         <v>6.69</v>
       </c>
-      <c r="E11" s="40">
+      <c r="E11" s="33">
         <v>7.41</v>
       </c>
-      <c r="F11" s="40">
+      <c r="F11" s="33">
         <v>8.81</v>
       </c>
-      <c r="G11" s="40">
+      <c r="G11" s="33">
         <v>340.39</v>
       </c>
-      <c r="H11" s="40">
+      <c r="H11" s="33">
         <v>2050</v>
       </c>
-      <c r="I11" s="40">
+      <c r="I11" s="33">
         <v>1371.913</v>
       </c>
-      <c r="J11" s="40">
+      <c r="J11" s="33">
         <v>5000.47</v>
       </c>
-      <c r="L11" s="36">
+      <c r="L11" s="29">
         <f>'[1]memoria GA'!$A$79</f>
         <v>0.91700000000000004</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="25"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="9" t="s">
         <v>19</v>
       </c>
@@ -1048,7 +1052,7 @@
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="36" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1082,13 +1086,13 @@
         <f>ESBMC!H11</f>
         <v>MO</v>
       </c>
-      <c r="L13" s="37">
+      <c r="L13" s="30">
         <f>ESBMC!L8</f>
         <v>0.91700000000000015</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="B14" s="23"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="3" t="s">
         <v>21</v>
       </c>
@@ -1118,47 +1122,47 @@
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="38" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="40">
+      <c r="D15" s="33">
         <f>'ESBMC-SS'!H6</f>
         <v>2.2023333333333333</v>
       </c>
-      <c r="E15" s="40">
+      <c r="E15" s="33">
         <f>'ESBMC-SS'!H5</f>
         <v>5.8263333333333334</v>
       </c>
-      <c r="F15" s="40">
+      <c r="F15" s="33">
         <f>'ESBMC-SS'!H7</f>
         <v>6.9750000000000005</v>
       </c>
-      <c r="G15" s="40">
+      <c r="G15" s="33">
         <f>'ESBMC-SS'!H8</f>
         <v>1609.3333333333333</v>
       </c>
-      <c r="H15" s="41" t="str">
+      <c r="H15" s="34" t="str">
         <f>'ESBMC-SS'!H9</f>
         <v>TO</v>
       </c>
-      <c r="I15" s="41" t="str">
+      <c r="I15" s="34" t="str">
         <f>'ESBMC-SS'!H10</f>
         <v>TO</v>
       </c>
-      <c r="J15" s="41" t="str">
+      <c r="J15" s="34" t="str">
         <f>'ESBMC-SS'!H11</f>
         <v>TO</v>
       </c>
-      <c r="L15" s="37">
+      <c r="L15" s="30">
         <f>'ESBMC-SS'!L9</f>
         <v>0.91700000000000004</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="B16" s="25"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="9" t="s">
         <v>21</v>
       </c>
@@ -1178,18 +1182,18 @@
         <f>'ESBMC-SS'!C8</f>
         <v>241</v>
       </c>
-      <c r="H16" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16" s="42" t="s">
+      <c r="H16" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="35" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="36" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1223,13 +1227,13 @@
         <f>'ESBMC-PS'!H11</f>
         <v>TO</v>
       </c>
-      <c r="L17" s="37">
+      <c r="L17" s="30">
         <f>'ESBMC-PS'!L9</f>
         <v>0.95849999999999991</v>
       </c>
     </row>
     <row r="18" spans="2:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="B18" s="23"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="3" t="s">
         <v>21</v>
       </c>
@@ -1260,47 +1264,47 @@
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="38" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="33">
         <f>'ESBMC-PB'!H6</f>
         <v>4.333333333333333</v>
       </c>
-      <c r="E19" s="40">
+      <c r="E19" s="33">
         <f>'ESBMC-PB'!H5</f>
         <v>4.666666666666667</v>
       </c>
-      <c r="F19" s="40">
+      <c r="F19" s="33">
         <f>'ESBMC-PB'!H7</f>
         <v>6.333333333333333</v>
       </c>
-      <c r="G19" s="40">
+      <c r="G19" s="33">
         <f>'ESBMC-PB'!H8</f>
         <v>218.66666666666666</v>
       </c>
-      <c r="H19" s="41" t="str">
+      <c r="H19" s="34" t="str">
         <f>'ESBMC-PB'!H9</f>
         <v>TO</v>
       </c>
-      <c r="I19" s="41" t="str">
+      <c r="I19" s="34" t="str">
         <f>'ESBMC-PB'!H10</f>
         <v>TO</v>
       </c>
-      <c r="J19" s="41" t="str">
+      <c r="J19" s="34" t="str">
         <f>'ESBMC-PB'!H11</f>
         <v>TO</v>
       </c>
-      <c r="L19" s="37">
+      <c r="L19" s="30">
         <f>'ESBMC-PB'!L9</f>
         <v>0.91700000000000004</v>
       </c>
     </row>
     <row r="20" spans="2:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="B20" s="25"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="9" t="s">
         <v>21</v>
       </c>
@@ -1320,18 +1324,18 @@
         <f>'ESBMC-PB'!C8</f>
         <v>241</v>
       </c>
-      <c r="H20" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="J20" s="42" t="s">
+      <c r="H20" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="35" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="36" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1365,13 +1369,13 @@
         <f>'ESBMC-vZ'!D11</f>
         <v>TO</v>
       </c>
-      <c r="L21" s="36">
+      <c r="L21" s="29">
         <f>'ESBMC-vZ'!L8</f>
         <v>0.91700000000000004</v>
       </c>
     </row>
     <row r="22" spans="2:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="B22" s="23"/>
+      <c r="B22" s="37"/>
       <c r="C22" s="3" t="s">
         <v>21</v>
       </c>
@@ -1423,6 +1427,685 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:L24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="6" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="9.140625" style="1"/>
+    <col min="12" max="12" width="21.5703125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E1" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C3" s="6"/>
+      <c r="D3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1">
+        <v>21</v>
+      </c>
+      <c r="F4" s="1">
+        <v>26</v>
+      </c>
+      <c r="G4" s="1">
+        <v>150</v>
+      </c>
+      <c r="H4" s="1">
+        <v>329</v>
+      </c>
+      <c r="I4" s="1">
+        <v>261</v>
+      </c>
+      <c r="J4" s="1">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1">
+        <v>32</v>
+      </c>
+      <c r="E5" s="1">
+        <v>48</v>
+      </c>
+      <c r="F5" s="1">
+        <v>69</v>
+      </c>
+      <c r="G5" s="1">
+        <v>331</v>
+      </c>
+      <c r="H5" s="1">
+        <v>448</v>
+      </c>
+      <c r="I5" s="1">
+        <v>422</v>
+      </c>
+      <c r="J5" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1">
+        <v>20</v>
+      </c>
+      <c r="G6" s="1">
+        <v>50</v>
+      </c>
+      <c r="H6" s="1">
+        <v>600</v>
+      </c>
+      <c r="I6" s="1">
+        <v>4578</v>
+      </c>
+      <c r="J6" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="B7" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="8">
+        <v>15</v>
+      </c>
+      <c r="E7" s="8">
+        <v>47</v>
+      </c>
+      <c r="F7" s="8">
+        <v>31</v>
+      </c>
+      <c r="G7" s="8">
+        <v>241</v>
+      </c>
+      <c r="H7" s="8">
+        <v>692</v>
+      </c>
+      <c r="I7" s="8">
+        <v>13820</v>
+      </c>
+      <c r="J7" s="8">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="B8" s="41"/>
+      <c r="C8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="9">
+        <v>19</v>
+      </c>
+      <c r="E8" s="9">
+        <v>4</v>
+      </c>
+      <c r="F8" s="9">
+        <v>19</v>
+      </c>
+      <c r="G8" s="9">
+        <v>46</v>
+      </c>
+      <c r="H8" s="9">
+        <v>533</v>
+      </c>
+      <c r="I8" s="9">
+        <v>4231</v>
+      </c>
+      <c r="J8" s="9">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1.57</v>
+      </c>
+      <c r="E9" s="15">
+        <v>1.27</v>
+      </c>
+      <c r="F9" s="15">
+        <v>1.61</v>
+      </c>
+      <c r="G9" s="15">
+        <v>648.9</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1806.2</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="29">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="B10" s="37"/>
+      <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="3">
+        <v>15</v>
+      </c>
+      <c r="E10" s="3">
+        <v>47</v>
+      </c>
+      <c r="F10" s="3">
+        <v>31</v>
+      </c>
+      <c r="G10" s="3">
+        <v>241</v>
+      </c>
+      <c r="H10" s="3">
+        <v>692</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="33">
+        <v>6.69</v>
+      </c>
+      <c r="E11" s="33">
+        <v>7.41</v>
+      </c>
+      <c r="F11" s="33">
+        <v>8.81</v>
+      </c>
+      <c r="G11" s="33">
+        <v>340.39</v>
+      </c>
+      <c r="H11" s="33">
+        <v>2050</v>
+      </c>
+      <c r="I11" s="33">
+        <v>1371.913</v>
+      </c>
+      <c r="J11" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="29">
+        <f>'[1]memoria GA'!$A$79</f>
+        <v>0.91700000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="39"/>
+      <c r="C12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="21">
+        <v>13.3</v>
+      </c>
+      <c r="E12" s="21">
+        <v>0</v>
+      </c>
+      <c r="F12" s="21">
+        <v>29</v>
+      </c>
+      <c r="G12" s="21">
+        <v>1.7</v>
+      </c>
+      <c r="H12" s="21">
+        <v>-6.5</v>
+      </c>
+      <c r="I12" s="21">
+        <v>-37.6</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="15">
+        <f>ESBMC!H6</f>
+        <v>30.333333333333332</v>
+      </c>
+      <c r="E13" s="15">
+        <f>ESBMC!H5</f>
+        <v>313.66666666666669</v>
+      </c>
+      <c r="F13" s="15">
+        <f>ESBMC!H7</f>
+        <v>324.66666666666669</v>
+      </c>
+      <c r="G13" s="4" t="str">
+        <f>ESBMC!H8</f>
+        <v>MO</v>
+      </c>
+      <c r="H13" s="4" t="str">
+        <f>ESBMC!H9</f>
+        <v>MO</v>
+      </c>
+      <c r="I13" s="4" t="str">
+        <f>ESBMC!H10</f>
+        <v>MO</v>
+      </c>
+      <c r="J13" s="4" t="str">
+        <f>ESBMC!H11</f>
+        <v>MO</v>
+      </c>
+      <c r="L13" s="30">
+        <f>ESBMC!L8</f>
+        <v>0.91700000000000015</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="B14" s="37"/>
+      <c r="C14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="3">
+        <f>ESBMC!C6</f>
+        <v>15</v>
+      </c>
+      <c r="E14" s="3">
+        <f>ESBMC!C5</f>
+        <v>47</v>
+      </c>
+      <c r="F14" s="3">
+        <f>ESBMC!C7</f>
+        <v>31</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="33">
+        <f>'ESBMC-SS'!H6</f>
+        <v>2.2023333333333333</v>
+      </c>
+      <c r="E15" s="33">
+        <f>'ESBMC-SS'!H5</f>
+        <v>5.8263333333333334</v>
+      </c>
+      <c r="F15" s="33">
+        <f>'ESBMC-SS'!H7</f>
+        <v>6.9750000000000005</v>
+      </c>
+      <c r="G15" s="33">
+        <f>'ESBMC-SS'!H8</f>
+        <v>1609.3333333333333</v>
+      </c>
+      <c r="H15" s="34" t="str">
+        <f>'ESBMC-SS'!H9</f>
+        <v>TO</v>
+      </c>
+      <c r="I15" s="34" t="str">
+        <f>'ESBMC-SS'!H10</f>
+        <v>TO</v>
+      </c>
+      <c r="J15" s="34" t="str">
+        <f>'ESBMC-SS'!H11</f>
+        <v>TO</v>
+      </c>
+      <c r="L15" s="30">
+        <f>'ESBMC-SS'!L9</f>
+        <v>0.91700000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="B16" s="39"/>
+      <c r="C16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="9">
+        <f>'ESBMC-SS'!C6</f>
+        <v>15</v>
+      </c>
+      <c r="E16" s="9">
+        <f>'ESBMC-SS'!C5</f>
+        <v>47</v>
+      </c>
+      <c r="F16" s="9">
+        <f>'ESBMC-SS'!C7</f>
+        <v>31</v>
+      </c>
+      <c r="G16" s="9">
+        <f>'ESBMC-SS'!C8</f>
+        <v>241</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="15">
+        <f>'ESBMC-PS'!H6</f>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="E17" s="15">
+        <f>'ESBMC-PS'!H5</f>
+        <v>10</v>
+      </c>
+      <c r="F17" s="15">
+        <f>'ESBMC-PS'!H7</f>
+        <v>12</v>
+      </c>
+      <c r="G17" s="15">
+        <f>'ESBMC-PS'!H8</f>
+        <v>2468</v>
+      </c>
+      <c r="H17" s="4" t="str">
+        <f>'ESBMC-PS'!H9</f>
+        <v>TO</v>
+      </c>
+      <c r="I17" s="4" t="str">
+        <f>'ESBMC-PS'!H10</f>
+        <v>TO</v>
+      </c>
+      <c r="J17" s="4" t="str">
+        <f>'ESBMC-PS'!H11</f>
+        <v>TO</v>
+      </c>
+      <c r="L17" s="30">
+        <f>'ESBMC-PS'!L9</f>
+        <v>0.95849999999999991</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="B18" s="37"/>
+      <c r="C18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="3">
+        <f>'ESBMC-PS'!C6</f>
+        <v>15</v>
+      </c>
+      <c r="E18" s="3">
+        <f>'ESBMC-PS'!C5</f>
+        <v>47</v>
+      </c>
+      <c r="F18" s="3">
+        <f>'ESBMC-PS'!C7</f>
+        <v>31</v>
+      </c>
+      <c r="G18" s="3">
+        <f>'ESBMC-PS'!C8</f>
+        <v>241</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="33">
+        <f>'ESBMC-PB'!H6</f>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="E19" s="33">
+        <f>'ESBMC-PB'!H5</f>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="F19" s="33">
+        <f>'ESBMC-PB'!H7</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="G19" s="33">
+        <f>'ESBMC-PB'!H8</f>
+        <v>218.66666666666666</v>
+      </c>
+      <c r="H19" s="34" t="str">
+        <f>'ESBMC-PB'!H9</f>
+        <v>TO</v>
+      </c>
+      <c r="I19" s="34" t="str">
+        <f>'ESBMC-PB'!H10</f>
+        <v>TO</v>
+      </c>
+      <c r="J19" s="34" t="str">
+        <f>'ESBMC-PB'!H11</f>
+        <v>TO</v>
+      </c>
+      <c r="L19" s="30">
+        <f>'ESBMC-PB'!L9</f>
+        <v>0.91700000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="B20" s="39"/>
+      <c r="C20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="9">
+        <f>'ESBMC-PB'!C6</f>
+        <v>15</v>
+      </c>
+      <c r="E20" s="9">
+        <f>'ESBMC-PB'!C5</f>
+        <v>47</v>
+      </c>
+      <c r="F20" s="9">
+        <f>'ESBMC-PB'!C7</f>
+        <v>31</v>
+      </c>
+      <c r="G20" s="9">
+        <f>'ESBMC-PB'!C8</f>
+        <v>241</v>
+      </c>
+      <c r="H20" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="15">
+        <f>'ESBMC-vZ'!H6</f>
+        <v>0.29458093643333333</v>
+      </c>
+      <c r="E21" s="15">
+        <f>'ESBMC-vZ'!H5</f>
+        <v>0.31701231000000002</v>
+      </c>
+      <c r="F21" s="15">
+        <f>'ESBMC-vZ'!H7</f>
+        <v>0.66174101829999998</v>
+      </c>
+      <c r="G21" s="15">
+        <f>'ESBMC-vZ'!H8</f>
+        <v>86.371642669999986</v>
+      </c>
+      <c r="H21" s="4" t="str">
+        <f>'ESBMC-vZ'!D9</f>
+        <v>TO</v>
+      </c>
+      <c r="I21" s="4" t="str">
+        <f>'ESBMC-vZ'!D10</f>
+        <v>TO</v>
+      </c>
+      <c r="J21" s="4" t="str">
+        <f>'ESBMC-vZ'!D11</f>
+        <v>TO</v>
+      </c>
+      <c r="L21" s="29">
+        <f>'ESBMC-vZ'!L8</f>
+        <v>0.91700000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="B22" s="37"/>
+      <c r="C22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="3">
+        <f>'ESBMC-vZ'!C6</f>
+        <v>15</v>
+      </c>
+      <c r="E22" s="3">
+        <f>'ESBMC-vZ'!C5</f>
+        <v>47</v>
+      </c>
+      <c r="F22" s="3">
+        <f>'ESBMC-vZ'!C7</f>
+        <v>31</v>
+      </c>
+      <c r="G22" s="3">
+        <f>'ESBMC-vZ'!C8</f>
+        <v>241</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H24" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M18"/>
   <sheetViews>
@@ -1459,13 +2142,13 @@
       <c r="L2" s="12"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="16"/>
@@ -1531,7 +2214,7 @@
       <c r="K5">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="L5" s="32">
+      <c r="L5" s="25">
         <f>1-K5</f>
         <v>0.91700000000000004</v>
       </c>
@@ -1571,7 +2254,7 @@
       <c r="K6">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="L6" s="32">
+      <c r="L6" s="25">
         <f>1-K6</f>
         <v>0.91700000000000004</v>
       </c>
@@ -1611,7 +2294,7 @@
       <c r="K7">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="L7" s="32">
+      <c r="L7" s="25">
         <f>1-K7</f>
         <v>0.91700000000000004</v>
       </c>
@@ -1627,19 +2310,19 @@
       <c r="C8" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="38" t="s">
+      <c r="H8" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="L8" s="35">
+      <c r="L8" s="28">
         <f>AVERAGE(L5:L7)</f>
         <v>0.91700000000000015</v>
       </c>
@@ -1651,16 +2334,16 @@
       <c r="C9" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="38" t="s">
+      <c r="H9" s="31" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1671,16 +2354,16 @@
       <c r="C10" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="29" t="s">
+      <c r="F10" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="38" t="s">
+      <c r="H10" s="31" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1691,16 +2374,16 @@
       <c r="C11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="38" t="s">
+      <c r="H11" s="31" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1721,7 +2404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M18"/>
   <sheetViews>
@@ -1756,13 +2439,13 @@
       <c r="L2" s="12"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="16"/>
@@ -1828,7 +2511,7 @@
       <c r="K5">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="L5" s="32">
+      <c r="L5" s="25">
         <f>1-K5</f>
         <v>0.91700000000000004</v>
       </c>
@@ -1868,7 +2551,7 @@
       <c r="K6">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="L6" s="32">
+      <c r="L6" s="25">
         <f>1-K6</f>
         <v>0.91700000000000004</v>
       </c>
@@ -1908,7 +2591,7 @@
       <c r="K7">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="L7" s="32">
+      <c r="L7" s="25">
         <f>1-K7</f>
         <v>0.91700000000000004</v>
       </c>
@@ -1924,13 +2607,13 @@
       <c r="C8" s="16">
         <v>241</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="24">
         <v>1605</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="24">
         <v>1620</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="24">
         <v>1603</v>
       </c>
       <c r="H8">
@@ -1948,7 +2631,7 @@
       <c r="K8">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="L8" s="32">
+      <c r="L8" s="25">
         <f>1-K8</f>
         <v>0.91700000000000004</v>
       </c>
@@ -1973,10 +2656,10 @@
       <c r="F9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" s="34">
+      <c r="H9" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="27">
         <f>AVERAGE(L5:L8)</f>
         <v>0.91700000000000004</v>
       </c>
@@ -1997,7 +2680,7 @@
       <c r="F10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="39" t="s">
+      <c r="H10" s="32" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2017,7 +2700,7 @@
       <c r="F11" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="32" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2039,7 +2722,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M18"/>
   <sheetViews>
@@ -2076,13 +2759,13 @@
       <c r="L2" s="12"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="16"/>
@@ -2187,7 +2870,7 @@
       <c r="K6">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="L6" s="32">
+      <c r="L6" s="25">
         <f>1-K6</f>
         <v>0.91700000000000004</v>
       </c>
@@ -2242,13 +2925,13 @@
       <c r="C8" s="16">
         <v>241</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="24">
         <v>2482</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="24">
         <v>2478</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="24">
         <v>2444</v>
       </c>
       <c r="H8">
@@ -2266,7 +2949,7 @@
       <c r="K8">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="L8" s="32">
+      <c r="L8" s="25">
         <f>1-K8</f>
         <v>0.91700000000000004</v>
       </c>
@@ -2291,10 +2974,10 @@
       <c r="F9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" s="33">
+      <c r="H9" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="26">
         <f>AVERAGE(L5:L8)</f>
         <v>0.95849999999999991</v>
       </c>
@@ -2315,7 +2998,7 @@
       <c r="F10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="39" t="s">
+      <c r="H10" s="32" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2335,326 +3018,7 @@
       <c r="F11" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="39" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="G16" s="13"/>
-    </row>
-    <row r="17" spans="7:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="G17" s="14"/>
-    </row>
-    <row r="18" spans="7:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="H18" s="14"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:F3"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10:H11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K2" s="11"/>
-      <c r="L2" s="12"/>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="16">
-        <v>47</v>
-      </c>
-      <c r="D5" s="16">
-        <v>5</v>
-      </c>
-      <c r="E5" s="16">
-        <v>4</v>
-      </c>
-      <c r="F5" s="16">
-        <v>5</v>
-      </c>
-      <c r="H5">
-        <f>AVERAGE(D5:F5)</f>
-        <v>4.666666666666667</v>
-      </c>
-      <c r="I5">
-        <f>_xlfn.STDEV.S(D5:F5)</f>
-        <v>0.57735026918962784</v>
-      </c>
-      <c r="J5">
-        <f>_xlfn.CONFIDENCE.NORM(K5,I5,3)</f>
-        <v>0.57784616794726706</v>
-      </c>
-      <c r="K5">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L5" s="32">
-        <f>1-K5</f>
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="M5" t="str">
-        <f>IF(I5&gt;J5,"NOK","OK")</f>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="16">
-        <v>15</v>
-      </c>
-      <c r="D6" s="16">
-        <v>5</v>
-      </c>
-      <c r="E6" s="16">
-        <v>4</v>
-      </c>
-      <c r="F6" s="16">
-        <v>4</v>
-      </c>
-      <c r="H6">
-        <f>AVERAGE(D6:F6)</f>
-        <v>4.333333333333333</v>
-      </c>
-      <c r="I6">
-        <f>_xlfn.STDEV.S(D6:F6)</f>
-        <v>0.57735026918962473</v>
-      </c>
-      <c r="J6">
-        <f>_xlfn.CONFIDENCE.NORM(K6,I6,3)</f>
-        <v>0.57784616794726396</v>
-      </c>
-      <c r="K6">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L6" s="32">
-        <f>1-K6</f>
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="M6" t="str">
-        <f>IF(I6&gt;J6,"NOK","OK")</f>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="16">
-        <v>31</v>
-      </c>
-      <c r="D7" s="16">
-        <v>7</v>
-      </c>
-      <c r="E7" s="16">
-        <v>6</v>
-      </c>
-      <c r="F7" s="16">
-        <v>6</v>
-      </c>
-      <c r="H7">
-        <f>AVERAGE(D7:F7)</f>
-        <v>6.333333333333333</v>
-      </c>
-      <c r="I7">
-        <f>_xlfn.STDEV.S(D7:F7)</f>
-        <v>0.57735026918962584</v>
-      </c>
-      <c r="J7">
-        <f>_xlfn.CONFIDENCE.NORM(K7,I7,3)</f>
-        <v>0.57784616794726507</v>
-      </c>
-      <c r="K7">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L7" s="32">
-        <f>1-K7</f>
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="M7" t="str">
-        <f>IF(I7&gt;J7,"NOK","OK")</f>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="16">
-        <v>241</v>
-      </c>
-      <c r="D8" s="30">
-        <v>215</v>
-      </c>
-      <c r="E8" s="30">
-        <v>220</v>
-      </c>
-      <c r="F8" s="30">
-        <v>221</v>
-      </c>
-      <c r="H8">
-        <f>AVERAGE(D8:F8)</f>
-        <v>218.66666666666666</v>
-      </c>
-      <c r="I8">
-        <f>_xlfn.STDEV.S(D8:F8)</f>
-        <v>3.2145502536643185</v>
-      </c>
-      <c r="J8">
-        <f>_xlfn.CONFIDENCE.NORM(K8,I8,3)</f>
-        <v>3.2173113010946741</v>
-      </c>
-      <c r="K8">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L8" s="32">
-        <f>1-K8</f>
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="M8" t="str">
-        <f>IF(I8&gt;J8,"NOK","OK")</f>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" s="34">
-        <f>AVERAGE(L5:L8)</f>
-        <v>0.91700000000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="39" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="32" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2712,13 +3076,13 @@
       <c r="L2" s="12"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
+      <c r="B3" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="16"/>
@@ -2761,6 +3125,325 @@
         <v>47</v>
       </c>
       <c r="D5" s="16">
+        <v>5</v>
+      </c>
+      <c r="E5" s="16">
+        <v>4</v>
+      </c>
+      <c r="F5" s="16">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <f>AVERAGE(D5:F5)</f>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="I5">
+        <f>_xlfn.STDEV.S(D5:F5)</f>
+        <v>0.57735026918962784</v>
+      </c>
+      <c r="J5">
+        <f>_xlfn.CONFIDENCE.NORM(K5,I5,3)</f>
+        <v>0.57784616794726706</v>
+      </c>
+      <c r="K5">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L5" s="25">
+        <f>1-K5</f>
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="M5" t="str">
+        <f>IF(I5&gt;J5,"NOK","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="16">
+        <v>15</v>
+      </c>
+      <c r="D6" s="16">
+        <v>5</v>
+      </c>
+      <c r="E6" s="16">
+        <v>4</v>
+      </c>
+      <c r="F6" s="16">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <f>AVERAGE(D6:F6)</f>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="I6">
+        <f>_xlfn.STDEV.S(D6:F6)</f>
+        <v>0.57735026918962473</v>
+      </c>
+      <c r="J6">
+        <f>_xlfn.CONFIDENCE.NORM(K6,I6,3)</f>
+        <v>0.57784616794726396</v>
+      </c>
+      <c r="K6">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L6" s="25">
+        <f>1-K6</f>
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="M6" t="str">
+        <f>IF(I6&gt;J6,"NOK","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="16">
+        <v>31</v>
+      </c>
+      <c r="D7" s="16">
+        <v>7</v>
+      </c>
+      <c r="E7" s="16">
+        <v>6</v>
+      </c>
+      <c r="F7" s="16">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <f>AVERAGE(D7:F7)</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="I7">
+        <f>_xlfn.STDEV.S(D7:F7)</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="J7">
+        <f>_xlfn.CONFIDENCE.NORM(K7,I7,3)</f>
+        <v>0.57784616794726507</v>
+      </c>
+      <c r="K7">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L7" s="25">
+        <f>1-K7</f>
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="M7" t="str">
+        <f>IF(I7&gt;J7,"NOK","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="16">
+        <v>241</v>
+      </c>
+      <c r="D8" s="23">
+        <v>215</v>
+      </c>
+      <c r="E8" s="23">
+        <v>220</v>
+      </c>
+      <c r="F8" s="23">
+        <v>221</v>
+      </c>
+      <c r="H8">
+        <f>AVERAGE(D8:F8)</f>
+        <v>218.66666666666666</v>
+      </c>
+      <c r="I8">
+        <f>_xlfn.STDEV.S(D8:F8)</f>
+        <v>3.2145502536643185</v>
+      </c>
+      <c r="J8">
+        <f>_xlfn.CONFIDENCE.NORM(K8,I8,3)</f>
+        <v>3.2173113010946741</v>
+      </c>
+      <c r="K8">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L8" s="25">
+        <f>1-K8</f>
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="M8" t="str">
+        <f>IF(I8&gt;J8,"NOK","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="27">
+        <f>AVERAGE(L5:L8)</f>
+        <v>0.91700000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="7:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="7:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="H18" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:M18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="11"/>
+      <c r="L2" s="12"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="16">
+        <v>47</v>
+      </c>
+      <c r="D5" s="16">
         <v>0.3183119297</v>
       </c>
       <c r="E5" s="16">
@@ -2784,7 +3467,7 @@
       <c r="K5">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="L5" s="32">
+      <c r="L5" s="25">
         <f>1-K5</f>
         <v>0.91700000000000004</v>
       </c>
@@ -2824,7 +3507,7 @@
       <c r="K6">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="L6" s="32">
+      <c r="L6" s="25">
         <f>1-K6</f>
         <v>0.91700000000000004</v>
       </c>
@@ -2864,7 +3547,7 @@
       <c r="K7">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="L7" s="32">
+      <c r="L7" s="25">
         <f>1-K7</f>
         <v>0.91700000000000004</v>
       </c>
@@ -2904,7 +3587,7 @@
       <c r="K8">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="L8" s="32">
+      <c r="L8" s="25">
         <f>1-K8</f>
         <v>0.91700000000000004</v>
       </c>
@@ -2929,10 +3612,10 @@
       <c r="F9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" s="34">
+      <c r="H9" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="27">
         <f>AVERAGE(L5:L8)</f>
         <v>0.91700000000000004</v>
       </c>
@@ -2953,7 +3636,7 @@
       <c r="F10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="39" t="s">
+      <c r="H10" s="32" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2973,7 +3656,7 @@
       <c r="F11" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="32" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>